<commit_message>
Atualização automática de IJUI.xlsx
</commit_message>
<xml_diff>
--- a/IJUI.xlsx
+++ b/IJUI.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gera-fichas\Comarcas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{20CC4867-871B-498E-8874-EE60100897AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{82069917-B4A9-429F-B324-CE0192BF26A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,20 +23,7 @@
     <sheet name="Recolhimento x Eliminacao" sheetId="7" r:id="rId8"/>
     <sheet name="Desarquivamentos Pendentes" sheetId="8" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -1206,7 +1193,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -1267,30 +1254,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="thin">
         <color indexed="64"/>
@@ -1308,7 +1271,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1347,17 +1310,12 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1405,7 +1363,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 3" xfId="1" xr:uid="{98256865-B18B-4E30-953E-05CB7538AF37}"/>
+    <cellStyle name="Normal 3" xfId="1" xr:uid="{B840DE14-FCE3-4B3F-97BD-E4DD97FC4419}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1435,10 +1393,10 @@
         <xdr:cNvPr id="2" name="Chart1" title="Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1E764868-68C6-4A77-9622-5CF9DDD8D59D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F74E3CBA-7595-4C57-9817-4AF33EA31D1F}"/>
             </a:ext>
             <a:ext uri="GoogleSheetsCustomDataVersion1">
-              <go:sheetsCustomData xmlns="" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:go="http://customooxmlschemas.google.com/" pictureOfChart="1"/>
+              <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="" pictureOfChart="1"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1476,7 +1434,7 @@
         <xdr:cNvPr id="3" name="Shape 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DD50AAF8-1DDA-4474-8F5B-403047B9EE11}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C13B9F04-9195-4522-9FD3-4EBE8231C562}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1539,7 +1497,7 @@
         <xdr:cNvPr id="4" name="Shape 2" title="Desenho">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4DE4586B-85D1-462C-999B-1FDC45C0F517}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{002815B2-A5D2-49BB-959E-BB4180CD2812}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1558,7 +1516,7 @@
           <xdr:cNvPr id="5" name="Shape 4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B18FB7C6-594A-BCB2-C96A-DB0D06F61BD1}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A0EEAA87-FD2D-4041-AB07-596228A28721}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1607,7 +1565,7 @@
           <xdr:cNvPr id="6" name="Shape 5">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7AB48858-BB93-2782-39D9-7C5572B4C72C}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9F5BBB74-1C86-11DE-7479-2BEF55B04496}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1626,7 +1584,7 @@
             <xdr:cNvPr id="7" name="Shape 6">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CED58B2B-5386-6880-4168-A40DF9F4BC10}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B63E1641-15A7-2AD7-2F95-5DCBC8AA4CD4}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1657,7 +1615,7 @@
             <xdr:cNvPr id="8" name="Shape 7">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5081267A-D582-D552-7818-8FFB9DA8068E}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5ABD0547-2262-2382-8D80-44F27C08DC95}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1688,7 +1646,7 @@
             <xdr:cNvPr id="9" name="Shape 8">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{17C38B27-6F5B-A4AB-72F0-B5C64D0A2E48}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BB2AFC76-00CF-5E20-6E9E-28D004DD5AB6}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1731,7 +1689,7 @@
         <xdr:cNvPr id="10" name="image2.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9015F8D0-30F4-4C4E-9471-3EF5D8C563C1}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{30FCB103-2A81-4585-8E4F-03FC7B08C3AF}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1769,7 +1727,7 @@
         <xdr:cNvPr id="11" name="image1.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{05678BC2-E95E-4D00-84AB-52A9B9B9385E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F907C019-EB88-4E07-812C-E7BCE0EC00F6}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1812,7 +1770,7 @@
         <xdr:cNvPr id="12" name="Imagem 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0C1E8BAE-721D-485A-BB35-F7C9B159338C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3DCD1317-9CCF-454D-9462-2CEE0615DE75}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2125,7 +2083,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E79A76A5-E526-4855-89DF-D045B2585DEA}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{274B818F-82D4-4562-A73D-DFA046AE0E67}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -2137,98 +2095,98 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="5" width="12.5703125" style="42"/>
-    <col min="6" max="6" width="2" style="42" customWidth="1"/>
-    <col min="7" max="16" width="13.42578125" style="42" customWidth="1"/>
-    <col min="17" max="16384" width="12.5703125" style="42"/>
+    <col min="1" max="5" width="12.5703125" style="39"/>
+    <col min="6" max="6" width="2" style="39" customWidth="1"/>
+    <col min="7" max="16" width="13.42578125" style="39" customWidth="1"/>
+    <col min="17" max="16384" width="12.5703125" style="39"/>
   </cols>
   <sheetData>
     <row r="1" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F1" s="41"/>
+      <c r="F1" s="38"/>
     </row>
     <row r="2" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F2" s="41"/>
+      <c r="F2" s="38"/>
     </row>
     <row r="3" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F3" s="41"/>
+      <c r="F3" s="38"/>
     </row>
     <row r="4" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F4" s="41"/>
+      <c r="F4" s="38"/>
     </row>
     <row r="5" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F5" s="41"/>
+      <c r="F5" s="38"/>
     </row>
     <row r="6" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F6" s="41"/>
+      <c r="F6" s="38"/>
     </row>
     <row r="7" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F7" s="41"/>
+      <c r="F7" s="38"/>
     </row>
     <row r="8" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F8" s="41"/>
+      <c r="F8" s="38"/>
     </row>
     <row r="9" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F9" s="41"/>
+      <c r="F9" s="38"/>
     </row>
     <row r="10" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F10" s="41"/>
+      <c r="F10" s="38"/>
     </row>
     <row r="11" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F11" s="41"/>
+      <c r="F11" s="38"/>
     </row>
     <row r="12" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F12" s="41"/>
+      <c r="F12" s="38"/>
     </row>
     <row r="13" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F13" s="41"/>
+      <c r="F13" s="38"/>
     </row>
     <row r="14" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F14" s="41"/>
+      <c r="F14" s="38"/>
     </row>
     <row r="15" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F15" s="41"/>
+      <c r="F15" s="38"/>
     </row>
     <row r="16" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F16" s="41"/>
+      <c r="F16" s="38"/>
     </row>
     <row r="17" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F17" s="41"/>
+      <c r="F17" s="38"/>
     </row>
     <row r="18" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F18" s="41"/>
+      <c r="F18" s="38"/>
     </row>
     <row r="19" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F19" s="41"/>
+      <c r="F19" s="38"/>
     </row>
     <row r="20" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F20" s="41"/>
+      <c r="F20" s="38"/>
     </row>
     <row r="21" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F21" s="41"/>
+      <c r="F21" s="38"/>
     </row>
     <row r="22" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F22" s="41"/>
+      <c r="F22" s="38"/>
     </row>
     <row r="23" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F23" s="41"/>
+      <c r="F23" s="38"/>
     </row>
     <row r="24" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F24" s="41"/>
+      <c r="F24" s="38"/>
     </row>
     <row r="25" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F25" s="41"/>
+      <c r="F25" s="38"/>
     </row>
     <row r="26" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F26" s="41"/>
+      <c r="F26" s="38"/>
     </row>
     <row r="27" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F27" s="41"/>
+      <c r="F27" s="38"/>
     </row>
     <row r="28" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F28" s="41"/>
+      <c r="F28" s="38"/>
     </row>
     <row r="29" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F29" s="41"/>
+      <c r="F29" s="38"/>
     </row>
   </sheetData>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -5556,19 +5514,19 @@
     <col min="2" max="2" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="16" t="s">
         <v>278</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="2" t="s">
         <v>279</v>
       </c>
     </row>
@@ -5602,46 +5560,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="18" t="s">
         <v>280</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="17" t="s">
         <v>281</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="D1" s="17" t="s">
         <v>282</v>
       </c>
-      <c r="E1" s="20" t="s">
+      <c r="E1" s="17" t="s">
         <v>283</v>
       </c>
-      <c r="F1" s="20" t="s">
+      <c r="F1" s="17" t="s">
         <v>284</v>
       </c>
-      <c r="G1" s="20" t="s">
+      <c r="G1" s="17" t="s">
         <v>285</v>
       </c>
-      <c r="H1" s="20" t="s">
+      <c r="H1" s="17" t="s">
         <v>286</v>
       </c>
-      <c r="I1" s="20" t="s">
+      <c r="I1" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="J1" s="20" t="s">
+      <c r="J1" s="17" t="s">
         <v>287</v>
       </c>
-      <c r="K1" s="20" t="s">
+      <c r="K1" s="17" t="s">
         <v>287</v>
       </c>
-      <c r="L1" s="20" t="s">
+      <c r="L1" s="17" t="s">
         <v>288</v>
       </c>
-      <c r="M1" s="20" t="s">
+      <c r="M1" s="17" t="s">
         <v>289</v>
       </c>
-      <c r="N1" s="20" t="s">
+      <c r="N1" s="17" t="s">
         <v>290</v>
       </c>
     </row>
@@ -5649,7 +5607,7 @@
       <c r="A2" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="B2" s="22">
+      <c r="B2" s="19">
         <v>441712</v>
       </c>
       <c r="C2" s="2" t="s">
@@ -5661,10 +5619,10 @@
       <c r="E2" s="2" t="s">
         <v>294</v>
       </c>
-      <c r="F2" s="23">
+      <c r="F2" s="20">
         <v>161.08000000000001</v>
       </c>
-      <c r="G2" s="23">
+      <c r="G2" s="20">
         <v>349</v>
       </c>
       <c r="H2" s="2" t="s">
@@ -5693,7 +5651,7 @@
       <c r="A3" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="B3" s="22">
+      <c r="B3" s="19">
         <v>441716</v>
       </c>
       <c r="C3" s="2" t="s">
@@ -5705,10 +5663,10 @@
       <c r="E3" s="2" t="s">
         <v>294</v>
       </c>
-      <c r="F3" s="23">
+      <c r="F3" s="20">
         <v>161.08000000000001</v>
       </c>
-      <c r="G3" s="23">
+      <c r="G3" s="20">
         <v>349</v>
       </c>
       <c r="H3" s="2" t="s">
@@ -5737,7 +5695,7 @@
       <c r="A4" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="B4" s="22">
+      <c r="B4" s="19">
         <v>453708</v>
       </c>
       <c r="C4" s="2" t="s">
@@ -5749,10 +5707,10 @@
       <c r="E4" s="2" t="s">
         <v>303</v>
       </c>
-      <c r="F4" s="23">
+      <c r="F4" s="20">
         <v>1444.81</v>
       </c>
-      <c r="G4" s="23">
+      <c r="G4" s="20">
         <v>2947.95</v>
       </c>
       <c r="H4" s="2" t="s">
@@ -5781,7 +5739,7 @@
       <c r="A5" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="B5" s="22">
+      <c r="B5" s="19">
         <v>453709</v>
       </c>
       <c r="C5" s="2" t="s">
@@ -5793,10 +5751,10 @@
       <c r="E5" s="2" t="s">
         <v>303</v>
       </c>
-      <c r="F5" s="23">
+      <c r="F5" s="20">
         <v>1444.81</v>
       </c>
-      <c r="G5" s="23">
+      <c r="G5" s="20">
         <v>2947.95</v>
       </c>
       <c r="H5" s="2" t="s">
@@ -5825,7 +5783,7 @@
       <c r="A6" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="B6" s="22">
+      <c r="B6" s="19">
         <v>438928</v>
       </c>
       <c r="C6" s="2" t="s">
@@ -5837,10 +5795,10 @@
       <c r="E6" s="2" t="s">
         <v>305</v>
       </c>
-      <c r="F6" s="23">
+      <c r="F6" s="20">
         <v>263.66000000000003</v>
       </c>
-      <c r="G6" s="23">
+      <c r="G6" s="20">
         <v>2636.55</v>
       </c>
       <c r="H6" s="2" t="s">
@@ -5869,7 +5827,7 @@
       <c r="A7" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="B7" s="22">
+      <c r="B7" s="19">
         <v>454791</v>
       </c>
       <c r="C7" s="2" t="s">
@@ -5881,10 +5839,10 @@
       <c r="E7" s="2" t="s">
         <v>309</v>
       </c>
-      <c r="F7" s="23">
+      <c r="F7" s="20">
         <v>238.52</v>
       </c>
-      <c r="G7" s="23">
+      <c r="G7" s="20">
         <v>299</v>
       </c>
       <c r="H7" s="2" t="s">
@@ -5913,7 +5871,7 @@
       <c r="A8" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="B8" s="22">
+      <c r="B8" s="19">
         <v>454792</v>
       </c>
       <c r="C8" s="2" t="s">
@@ -5925,10 +5883,10 @@
       <c r="E8" s="2" t="s">
         <v>309</v>
       </c>
-      <c r="F8" s="23">
+      <c r="F8" s="20">
         <v>238.52</v>
       </c>
-      <c r="G8" s="23">
+      <c r="G8" s="20">
         <v>299</v>
       </c>
       <c r="H8" s="2" t="s">
@@ -5957,7 +5915,7 @@
       <c r="A9" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="B9" s="22">
+      <c r="B9" s="19">
         <v>454793</v>
       </c>
       <c r="C9" s="2" t="s">
@@ -5969,10 +5927,10 @@
       <c r="E9" s="2" t="s">
         <v>311</v>
       </c>
-      <c r="F9" s="23">
+      <c r="F9" s="20">
         <v>415.9</v>
       </c>
-      <c r="G9" s="23">
+      <c r="G9" s="20">
         <v>521.20000000000005</v>
       </c>
       <c r="H9" s="2" t="s">
@@ -6001,7 +5959,7 @@
       <c r="A10" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="B10" s="22">
+      <c r="B10" s="19">
         <v>454794</v>
       </c>
       <c r="C10" s="2" t="s">
@@ -6013,10 +5971,10 @@
       <c r="E10" s="2" t="s">
         <v>311</v>
       </c>
-      <c r="F10" s="23">
+      <c r="F10" s="20">
         <v>415.9</v>
       </c>
-      <c r="G10" s="23">
+      <c r="G10" s="20">
         <v>521.20000000000005</v>
       </c>
       <c r="H10" s="2" t="s">
@@ -6045,7 +6003,7 @@
       <c r="A11" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="B11" s="22">
+      <c r="B11" s="19">
         <v>454795</v>
       </c>
       <c r="C11" s="2" t="s">
@@ -6057,10 +6015,10 @@
       <c r="E11" s="2" t="s">
         <v>311</v>
       </c>
-      <c r="F11" s="23">
+      <c r="F11" s="20">
         <v>415.9</v>
       </c>
-      <c r="G11" s="23">
+      <c r="G11" s="20">
         <v>521.20000000000005</v>
       </c>
       <c r="H11" s="2" t="s">
@@ -6089,7 +6047,7 @@
       <c r="A12" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="B12" s="22">
+      <c r="B12" s="19">
         <v>454796</v>
       </c>
       <c r="C12" s="2" t="s">
@@ -6101,10 +6059,10 @@
       <c r="E12" s="2" t="s">
         <v>311</v>
       </c>
-      <c r="F12" s="23">
+      <c r="F12" s="20">
         <v>415.9</v>
       </c>
-      <c r="G12" s="23">
+      <c r="G12" s="20">
         <v>521.20000000000005</v>
       </c>
       <c r="H12" s="2" t="s">
@@ -6133,7 +6091,7 @@
       <c r="A13" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="B13" s="22">
+      <c r="B13" s="19">
         <v>454797</v>
       </c>
       <c r="C13" s="2" t="s">
@@ -6145,10 +6103,10 @@
       <c r="E13" s="2" t="s">
         <v>311</v>
       </c>
-      <c r="F13" s="23">
+      <c r="F13" s="20">
         <v>415.9</v>
       </c>
-      <c r="G13" s="23">
+      <c r="G13" s="20">
         <v>521.20000000000005</v>
       </c>
       <c r="H13" s="2" t="s">
@@ -6177,7 +6135,7 @@
       <c r="A14" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="B14" s="22">
+      <c r="B14" s="19">
         <v>454798</v>
       </c>
       <c r="C14" s="2" t="s">
@@ -6189,10 +6147,10 @@
       <c r="E14" s="2" t="s">
         <v>311</v>
       </c>
-      <c r="F14" s="23">
+      <c r="F14" s="20">
         <v>415.9</v>
       </c>
-      <c r="G14" s="23">
+      <c r="G14" s="20">
         <v>521.20000000000005</v>
       </c>
       <c r="H14" s="2" t="s">
@@ -6221,7 +6179,7 @@
       <c r="A15" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="B15" s="22">
+      <c r="B15" s="19">
         <v>454799</v>
       </c>
       <c r="C15" s="2" t="s">
@@ -6233,10 +6191,10 @@
       <c r="E15" s="2" t="s">
         <v>311</v>
       </c>
-      <c r="F15" s="23">
+      <c r="F15" s="20">
         <v>415.9</v>
       </c>
-      <c r="G15" s="23">
+      <c r="G15" s="20">
         <v>521.20000000000005</v>
       </c>
       <c r="H15" s="2" t="s">
@@ -6265,7 +6223,7 @@
       <c r="A16" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="B16" s="22">
+      <c r="B16" s="19">
         <v>454800</v>
       </c>
       <c r="C16" s="2" t="s">
@@ -6277,10 +6235,10 @@
       <c r="E16" s="2" t="s">
         <v>311</v>
       </c>
-      <c r="F16" s="23">
+      <c r="F16" s="20">
         <v>415.9</v>
       </c>
-      <c r="G16" s="23">
+      <c r="G16" s="20">
         <v>521.20000000000005</v>
       </c>
       <c r="H16" s="2" t="s">
@@ -6309,7 +6267,7 @@
       <c r="A17" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="B17" s="22">
+      <c r="B17" s="19">
         <v>461001</v>
       </c>
       <c r="C17" s="2" t="s">
@@ -6321,10 +6279,10 @@
       <c r="E17" s="2" t="s">
         <v>311</v>
       </c>
-      <c r="F17" s="23">
+      <c r="F17" s="20">
         <v>415.9</v>
       </c>
-      <c r="G17" s="23">
+      <c r="G17" s="20">
         <v>521.20000000000005</v>
       </c>
       <c r="H17" s="2" t="s">
@@ -6353,7 +6311,7 @@
       <c r="A18" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="B18" s="22">
+      <c r="B18" s="19">
         <v>461002</v>
       </c>
       <c r="C18" s="2" t="s">
@@ -6365,10 +6323,10 @@
       <c r="E18" s="2" t="s">
         <v>311</v>
       </c>
-      <c r="F18" s="23">
+      <c r="F18" s="20">
         <v>415.9</v>
       </c>
-      <c r="G18" s="23">
+      <c r="G18" s="20">
         <v>521.20000000000005</v>
       </c>
       <c r="H18" s="2" t="s">
@@ -6407,14 +6365,14 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29.42578125" customWidth="1"/>
-    <col min="2" max="2" width="69.5703125" customWidth="1"/>
+    <col min="2" max="2" width="74.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="17" t="s">
         <v>312</v>
       </c>
     </row>
@@ -6445,68 +6403,68 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="22" t="s">
         <v>313</v>
       </c>
-      <c r="C1" s="24" t="s">
+      <c r="C1" s="21" t="s">
         <v>314</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="24" t="s">
         <v>315</v>
       </c>
-      <c r="C2" s="26" t="s">
+      <c r="C2" s="23" t="s">
         <v>316</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="27" t="s">
+      <c r="B3" s="24" t="s">
         <v>317</v>
       </c>
-      <c r="C3" s="26" t="s">
+      <c r="C3" s="23" t="s">
         <v>318</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="26" t="s">
+      <c r="A4" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="27" t="s">
+      <c r="B4" s="24" t="s">
         <v>319</v>
       </c>
-      <c r="C4" s="26" t="s">
+      <c r="C4" s="23" t="s">
         <v>318</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="26" t="s">
+      <c r="A5" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="27" t="s">
+      <c r="B5" s="24" t="s">
         <v>320</v>
       </c>
-      <c r="C5" s="26" t="s">
+      <c r="C5" s="23" t="s">
         <v>318</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="26" t="s">
+      <c r="A6" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="26" t="s">
+      <c r="B6" s="23" t="s">
         <v>321</v>
       </c>
-      <c r="C6" s="26" t="s">
+      <c r="C6" s="23" t="s">
         <v>316</v>
       </c>
     </row>
@@ -6531,54 +6489,55 @@
     <col min="6" max="6" width="12.5703125" customWidth="1"/>
     <col min="7" max="7" width="13" customWidth="1"/>
     <col min="8" max="8" width="15.42578125" customWidth="1"/>
-    <col min="9" max="14" width="13" customWidth="1"/>
-    <col min="15" max="15" width="30.85546875" customWidth="1"/>
+    <col min="9" max="12" width="13" customWidth="1"/>
+    <col min="13" max="13" width="42.140625" customWidth="1"/>
+    <col min="14" max="15" width="13" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="25" t="s">
         <v>322</v>
       </c>
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="26" t="s">
         <v>323</v>
       </c>
-      <c r="C1" s="29" t="s">
+      <c r="C1" s="26" t="s">
         <v>324</v>
       </c>
-      <c r="D1" s="29" t="s">
+      <c r="D1" s="26" t="s">
         <v>325</v>
       </c>
-      <c r="E1" s="29" t="s">
+      <c r="E1" s="26" t="s">
         <v>326</v>
       </c>
-      <c r="F1" s="30" t="s">
+      <c r="F1" s="27" t="s">
         <v>327</v>
       </c>
-      <c r="G1" s="30" t="s">
+      <c r="G1" s="27" t="s">
         <v>328</v>
       </c>
-      <c r="H1" s="28" t="s">
+      <c r="H1" s="25" t="s">
         <v>329</v>
       </c>
-      <c r="I1" s="28" t="s">
+      <c r="I1" s="25" t="s">
         <v>330</v>
       </c>
-      <c r="J1" s="28" t="s">
+      <c r="J1" s="25" t="s">
         <v>331</v>
       </c>
-      <c r="K1" s="28" t="s">
+      <c r="K1" s="25" t="s">
         <v>332</v>
       </c>
-      <c r="L1" s="28" t="s">
+      <c r="L1" s="25" t="s">
         <v>333</v>
       </c>
-      <c r="M1" s="28" t="s">
+      <c r="M1" s="25" t="s">
         <v>334</v>
       </c>
-      <c r="N1" s="28" t="s">
+      <c r="N1" s="25" t="s">
         <v>335</v>
       </c>
-      <c r="O1" s="28" t="s">
+      <c r="O1" s="25" t="s">
         <v>336</v>
       </c>
     </row>
@@ -6589,43 +6548,43 @@
       <c r="B2" s="2" t="s">
         <v>337</v>
       </c>
-      <c r="C2" s="31">
+      <c r="C2" s="28">
         <v>45748</v>
       </c>
-      <c r="D2" s="32">
+      <c r="D2" s="29">
         <v>7304</v>
       </c>
-      <c r="E2" s="32" t="s">
+      <c r="E2" s="29" t="s">
         <v>338</v>
       </c>
-      <c r="F2" s="33">
+      <c r="F2" s="30">
         <v>34537</v>
       </c>
-      <c r="G2" s="33">
+      <c r="G2" s="30">
         <v>4456</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>339</v>
       </c>
-      <c r="I2" s="34" t="s">
+      <c r="I2" s="31" t="s">
         <v>340</v>
       </c>
-      <c r="J2" s="34" t="s">
+      <c r="J2" s="31" t="s">
         <v>340</v>
       </c>
-      <c r="K2" s="34" t="s">
+      <c r="K2" s="31" t="s">
         <v>340</v>
       </c>
-      <c r="L2" s="34" t="s">
+      <c r="L2" s="31" t="s">
         <v>340</v>
       </c>
-      <c r="M2" s="35" t="s">
+      <c r="M2" s="32" t="s">
         <v>341</v>
       </c>
       <c r="N2" s="2" t="s">
         <v>339</v>
       </c>
-      <c r="O2" s="35" t="s">
+      <c r="O2" s="32" t="s">
         <v>341</v>
       </c>
     </row>
@@ -6656,25 +6615,24 @@
       <c r="B1" s="1" t="s">
         <v>342</v>
       </c>
-      <c r="C1" s="36" t="s">
+      <c r="C1" s="33" t="s">
         <v>343</v>
       </c>
-      <c r="E1" s="37">
-        <f>SUM(B2:B157)</f>
+      <c r="E1" s="34">
+        <v>15072</v>
+      </c>
+      <c r="F1" s="35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="36" t="s">
+        <v>291</v>
+      </c>
+      <c r="B2" s="37">
         <v>53</v>
       </c>
-      <c r="F1" s="38">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="39" t="s">
-        <v>291</v>
-      </c>
-      <c r="B2" s="40">
-        <v>53</v>
-      </c>
-      <c r="C2" s="38">
+      <c r="C2" s="35">
         <v>3.504827403782568E-3</v>
       </c>
     </row>

</xml_diff>